<commit_message>
[faet] 스킬 MP 감소
</commit_message>
<xml_diff>
--- a/excel2json-master/PlayerSkill_Data.xlsx
+++ b/excel2json-master/PlayerSkill_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952382B5-4CD1-4E8A-B325-92D85FC4999C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AF296-068A-40AF-90A7-BDFD0B0EBCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E541560-C0DE-451A-86CF-CC8DC2B3191B}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="22020" windowHeight="12336" xr2:uid="{8E541560-C0DE-451A-86CF-CC8DC2B3191B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>#PlayerSkill[{}]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>데미지를 준다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackAngle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,7 +608,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -638,9 +650,15 @@
       <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12">
@@ -658,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="7">
         <v>5</v>
@@ -666,9 +684,15 @@
       <c r="H2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="I2" s="4">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2</v>
+      </c>
+      <c r="K2" s="5">
+        <v>45</v>
+      </c>
       <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
@@ -685,7 +709,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="7">
         <v>10</v>
@@ -693,8 +717,15 @@
       <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="6"/>
+      <c r="I3" s="4">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="K3" s="6">
+        <v>100</v>
+      </c>
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1">
@@ -711,7 +742,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="7">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G4" s="7">
         <v>15</v>
@@ -719,8 +750,15 @@
       <c r="H4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="I4" s="4">
+        <v>4</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>90</v>
+      </c>
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1">
@@ -737,13 +775,22 @@
         <v>10</v>
       </c>
       <c r="F5" s="7">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G5" s="7">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>27</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5</v>
+      </c>
+      <c r="J5" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="K5" s="7">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1">
@@ -768,6 +815,15 @@
       <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5">
+        <v>2</v>
+      </c>
+      <c r="K6" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1">
       <c r="B7" s="5">
@@ -791,6 +847,15 @@
       <c r="H7" s="11" t="s">
         <v>1</v>
       </c>
+      <c r="I7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1">
       <c r="B8" s="5">
@@ -814,6 +879,15 @@
       <c r="H8" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="I8" s="4">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1">
       <c r="B9" s="5">
@@ -837,6 +911,15 @@
       <c r="H9" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="I9" s="4">
+        <v>3</v>
+      </c>
+      <c r="J9" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="K9" s="7">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1">
       <c r="B10" s="5">
@@ -860,6 +943,15 @@
       <c r="H10" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="I10" s="4">
+        <v>3</v>
+      </c>
+      <c r="J10" s="7">
+        <v>10</v>
+      </c>
+      <c r="K10" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="4" customFormat="1">
       <c r="B11" s="5">
@@ -882,6 +974,15 @@
       </c>
       <c r="H11" s="12" t="s">
         <v>3</v>
+      </c>
+      <c r="I11" s="4">
+        <v>3</v>
+      </c>
+      <c r="J11" s="7">
+        <v>10</v>
+      </c>
+      <c r="K11" s="7">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1">

</xml_diff>